<commit_message>
Corrige .gitignore e remove arquivos rastreados indevidamente
</commit_message>
<xml_diff>
--- a/input/cadastro_equipamentos.xlsx
+++ b/input/cadastro_equipamentos.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\NOTE_TI_CARLOS\Projetos_py\relatorio_equipamentos\input\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\NOTE_TI_CARLOS\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="162" uniqueCount="142">
   <si>
     <t>Loja</t>
   </si>
@@ -29,9 +29,6 @@
     <t>Equipamento</t>
   </si>
   <si>
-    <t>Notebook</t>
-  </si>
-  <si>
     <t>Quantidade</t>
   </si>
   <si>
@@ -62,31 +59,394 @@
     <t>5) Salve uma cópia preenchida em /input e o script irá gerar relatórios por loja em /output.</t>
   </si>
   <si>
-    <t xml:space="preserve">Notebook Samsung book </t>
-  </si>
-  <si>
-    <t>Notebook Samsung book 02</t>
-  </si>
-  <si>
-    <t>Impressora Epson L3250</t>
-  </si>
-  <si>
-    <t>Monitor HQ 24'</t>
-  </si>
-  <si>
-    <t>Roteador Intelbras</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Nobreak 1200 intelbras </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Nobreak 600 intelbras </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Switch Giga 8 portas </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Switch Giga 16 portas </t>
+    <t>IMPRESSORA BEMATECH MP-4200HS</t>
+  </si>
+  <si>
+    <t>IMPRESSORA ZEBRA ZD-220</t>
+  </si>
+  <si>
+    <t>IMPRESSORA ZEBRA ZD-230</t>
+  </si>
+  <si>
+    <t>DVR INTELBRAS 16 CANAIS 4TB</t>
+  </si>
+  <si>
+    <t>AMPLIFICADOR KT-705</t>
+  </si>
+  <si>
+    <t>AMPLIFICADOR LELONG LE-705</t>
+  </si>
+  <si>
+    <t>AR CONDICIONADO CARRIER</t>
+  </si>
+  <si>
+    <t>AR CONDICIONADO GREE (33K BTU'S)</t>
+  </si>
+  <si>
+    <t>AR CONDICIONADO SPRINGER MIDEA (33K BTUS)</t>
+  </si>
+  <si>
+    <t>CÂMERA DOME INTELBRAS 1120 D</t>
+  </si>
+  <si>
+    <t>CÂMERAS VIP BULLET</t>
+  </si>
+  <si>
+    <t>COMPUTADOR I3 1ª 6GB RAM</t>
+  </si>
+  <si>
+    <t>COMPUTADOR I3 1ª GEN 6GB</t>
+  </si>
+  <si>
+    <t>COMPUTADOR I5 2ª GEN 8GB</t>
+  </si>
+  <si>
+    <t>COMPUTADOR I5 6ª 6GB RAM</t>
+  </si>
+  <si>
+    <t>COMPUTADOR I7 2ª GEN 16GB</t>
+  </si>
+  <si>
+    <t>COMPUTADOR I7 6ª 16GB RAM</t>
+  </si>
+  <si>
+    <t>COMPUTADOR I7 6ª GEN 8GB</t>
+  </si>
+  <si>
+    <t>COMPUTADOR I7 6ª GEN 16GB</t>
+  </si>
+  <si>
+    <t>COMPUTADOR PC COM GARANTIA ATE DEZEMBRO</t>
+  </si>
+  <si>
+    <t>COMPUTADOR PC GENÉRICO I3 DE 1ª GERA COM 6GB</t>
+  </si>
+  <si>
+    <t>COMPUTADOR PC GENÉRICO I3 DE 3ª GERA COM 4GB</t>
+  </si>
+  <si>
+    <t>COMPUTADOR PC GENÉRICO I7-3ª GEN COM 16 GB</t>
+  </si>
+  <si>
+    <t>COMPUTADOR PC GENÉRICO I7-4ª GEN COM 16 GB</t>
+  </si>
+  <si>
+    <t>DVR 1016 C INTELBRAS</t>
+  </si>
+  <si>
+    <t>DVR INTELBRAS 16 CANAIS</t>
+  </si>
+  <si>
+    <t>DVR INTELBRAS 8 CANAIS</t>
+  </si>
+  <si>
+    <t>DVR INTELBRAS 8 CANAIS HD 2TB</t>
+  </si>
+  <si>
+    <t>ESTABILIZADOR (300 KVA)</t>
+  </si>
+  <si>
+    <t>IMPRESSORA BEMATECH MP-4200TH ADV</t>
+  </si>
+  <si>
+    <t>IMPRESSORA BROTHER MFC-L6902DW</t>
+  </si>
+  <si>
+    <t>IMPRESSORA DCP-L2540DW</t>
+  </si>
+  <si>
+    <t>IMPRESSORA EPSON TM-T20X</t>
+  </si>
+  <si>
+    <t>IMPRESSORA HP MPF 135A</t>
+  </si>
+  <si>
+    <t>IMPRESSORA MFP 432F DN</t>
+  </si>
+  <si>
+    <t>LEITOR CÓDIGO DE BARRAS WD-BT66 BLUETOOTH</t>
+  </si>
+  <si>
+    <t>MONITOR PRIZI 19”</t>
+  </si>
+  <si>
+    <t>MOTO G54 256GB</t>
+  </si>
+  <si>
+    <t>MOTO G54 265GB</t>
+  </si>
+  <si>
+    <t>NO BREAK 1200VA</t>
+  </si>
+  <si>
+    <t>NO BREAK 1200VA GENÉRICO</t>
+  </si>
+  <si>
+    <t>NO BREAK 1200VA RAGTECH</t>
+  </si>
+  <si>
+    <t>NO BREAK 1200VA USADO</t>
+  </si>
+  <si>
+    <t>NO BREAK ANTIGO APC 1200VA</t>
+  </si>
+  <si>
+    <t>NO BREAK APC 1200VA</t>
+  </si>
+  <si>
+    <t>NO BREAK APC 600VA</t>
+  </si>
+  <si>
+    <t>NO BREAK DE 1200 USADO</t>
+  </si>
+  <si>
+    <t>NO BREAK INTELBRAS 1200VA</t>
+  </si>
+  <si>
+    <t>NO BREAK INTELBRAS NOVO 1200VA</t>
+  </si>
+  <si>
+    <t>NO BREAK NHS MINI III</t>
+  </si>
+  <si>
+    <t>NO BREAK TS SHARA 1200VA</t>
+  </si>
+  <si>
+    <t>NO BREAK TS SHARA 1200 VA</t>
+  </si>
+  <si>
+    <t>NOTEBOOK ACER ASPIRE 5</t>
+  </si>
+  <si>
+    <t>NOTEBOOK SAMSUNG BOOK (I5 11ª 8GB) NP550XDA-KF4BR</t>
+  </si>
+  <si>
+    <t>NOTEBOOK SAMSUNG BOOK CORE I5 11ª 8GB</t>
+  </si>
+  <si>
+    <t>PC GENÉRICO I3 DE 1ª GERA COM 6GB</t>
+  </si>
+  <si>
+    <t>PC GENÉRICO I7 DE 2ª GERA COM 6GB</t>
+  </si>
+  <si>
+    <t>PC GENÉRICO I7 DE 3ª GERA COM 16 GB</t>
+  </si>
+  <si>
+    <t>PC GENÉRICO I7 DE 4ª GERA COM 16 GB</t>
+  </si>
+  <si>
+    <t>PC I7 2ª GERAÇÃO 16GB</t>
+  </si>
+  <si>
+    <t>RADIO AMADOR BAOFENG BF-777S</t>
+  </si>
+  <si>
+    <t>REDMI NOTE 14 5G</t>
+  </si>
+  <si>
+    <t>ROTEADOR INTELBRAS W5-1200GS</t>
+  </si>
+  <si>
+    <t>ROTEADOR MULTILASER MESH GIGA AX1.800</t>
+  </si>
+  <si>
+    <t>SAMSUNG GALAXY A11 (TELA TRINCADA)</t>
+  </si>
+  <si>
+    <t>SAMSUNG GALAXY A33</t>
+  </si>
+  <si>
+    <t>SAMSUNG GALAXY A34</t>
+  </si>
+  <si>
+    <t>SAMSUNG GALAXY BOOK CORE I5 11ª GEN 8GB</t>
+  </si>
+  <si>
+    <t>SAMSUNG GALAXY A05 128GB</t>
+  </si>
+  <si>
+    <t>SENSOR (PAT5001)</t>
+  </si>
+  <si>
+    <t>SENSOR FVP 5001 PET PRO</t>
+  </si>
+  <si>
+    <t>SENSOR IVP 5001 PET</t>
+  </si>
+  <si>
+    <t>SENSOR IVP 5301 PET PRO</t>
+  </si>
+  <si>
+    <t>SENSOR PET INTELBRAS 5001</t>
+  </si>
+  <si>
+    <t>SWITCH 8 PORTAS 5G 800Q+</t>
+  </si>
+  <si>
+    <t>SWITCH 8 PORTAS INTELBRAS GIGA</t>
+  </si>
+  <si>
+    <t>SWITCH 8 PORTAS INTELBRAS SG800Q+</t>
+  </si>
+  <si>
+    <t>TABLET REDMI PAD SE 256GB</t>
+  </si>
+  <si>
+    <t>TELEFONE SEM FIO TS3113 INTELBRAS</t>
+  </si>
+  <si>
+    <t>TRANSFORMADOR (1500KVA)</t>
+  </si>
+  <si>
+    <t>TRANSFORMADOR DE 5000VA</t>
+  </si>
+  <si>
+    <t>TRANSFORMADOR VOLTPRO 5000VA</t>
+  </si>
+  <si>
+    <t>IMPRESSORA BEMATECH MP-4200-TH</t>
+  </si>
+  <si>
+    <t>MINI PC DELL OPTIFLEX 3080 (I5 10ª ) 8GB RAM</t>
+  </si>
+  <si>
+    <t>MINI PC DELL OPTIFLEX 3000 (I5 12ª) GEN 8GB</t>
+  </si>
+  <si>
+    <t>MINI PC DELL OPTIFLEX 3080 (I5 10ª) 8GB RAM</t>
+  </si>
+  <si>
+    <t>MINI PC DELL OPTIFLEX 7020 (I5 14ª) GEN 16GB</t>
+  </si>
+  <si>
+    <t>SAMSUNG GALAXY A13 - SM-A135/ DM 4GB</t>
+  </si>
+  <si>
+    <t>LEITOR DE CÓDIGOS DE BARRA USB</t>
+  </si>
+  <si>
+    <t>MOTO G54 8GB</t>
+  </si>
+  <si>
+    <t>NOTEBOOK ACER ASPIRE 5 A515-54</t>
+  </si>
+  <si>
+    <t>MINI PC DELL PC DELL OPTIFLEX 3050 I3 7ª GEN 4GB</t>
+  </si>
+  <si>
+    <t>MINI PC DELL OPTIPLEX 3080 INTEL I5- 10ª G 8GB</t>
+  </si>
+  <si>
+    <t>NOTE DELL ISPIRON 5566 I5- 7ª GERA 8GB E 2 GB DE VÍDEO</t>
+  </si>
+  <si>
+    <t>SAMSUNG GALAXY BOOK 2 - CORE I5 12TH GEN 8GB</t>
+  </si>
+  <si>
+    <t>COMPUTADOR I7 7ª GEN COM 16GB</t>
+  </si>
+  <si>
+    <t>CÂMERAS VIP DOME</t>
+  </si>
+  <si>
+    <t>MONITOR 24''</t>
+  </si>
+  <si>
+    <t>SAMSUNG GALAXY A15 4GB</t>
+  </si>
+  <si>
+    <t>SAMSUNG GALAXY A13 4GB</t>
+  </si>
+  <si>
+    <t>SAMSUNG GALAXY S8+ 4GB CÉLIA</t>
+  </si>
+  <si>
+    <t>SAMSUNG GALAXY A01 (CELULAR LOJA)</t>
+  </si>
+  <si>
+    <t>CENTRAL INTELBRAS AMN24 NET</t>
+  </si>
+  <si>
+    <t>CENTRAL INTELBRAS ELC5001</t>
+  </si>
+  <si>
+    <t>COMPUTADOR I7 DE 2ª GEN 16GB</t>
+  </si>
+  <si>
+    <t>COMPUTADOR I7 DE 2ª GEN 6GB</t>
+  </si>
+  <si>
+    <t>SAMSUNG GALAXY BOOK 2 I5 12TH GEN - 8GB</t>
+  </si>
+  <si>
+    <t>SAMSUNG GALAXY A33 - MOB</t>
+  </si>
+  <si>
+    <t>MOTOG22 (CELULAR DE LOJA)</t>
+  </si>
+  <si>
+    <t>NOTEBOOK DELL PENTIUM 5405-U 8GB</t>
+  </si>
+  <si>
+    <t>SAMSUNG GALAXY A05 4GB RAM</t>
+  </si>
+  <si>
+    <t>SAMSUNG GALAXY A15 5G</t>
+  </si>
+  <si>
+    <t>SAMSUNG GALAXY A55 DE 4GB</t>
+  </si>
+  <si>
+    <t>IMPRESSORA HP LASER MFP 432 FDN</t>
+  </si>
+  <si>
+    <t>ROTEADOR INTELBRAS W5-1200F</t>
+  </si>
+  <si>
+    <t>ROTEADOR INTELBRAS W5-1200G</t>
+  </si>
+  <si>
+    <t>MINI PC DELL OPTIPLEX 3070 I5-9ª GEN 16GB</t>
+  </si>
+  <si>
+    <t>MINI PC DELL OPTIPLEX 3080 I3 8ª GEN 4GB</t>
+  </si>
+  <si>
+    <t>MINI PC DELL OPTIPLEX 3080 I3-10ª GEN 8 GB</t>
+  </si>
+  <si>
+    <t>MINI PC DELL OPTIPLEX 3060 I3 8ª GEN 4GB</t>
+  </si>
+  <si>
+    <t>MINI PC DELL OPTIPLEX 3070 CORE I3 - 9ª GEN 8GB</t>
+  </si>
+  <si>
+    <t>ROTEADOR INTELBRAS AC 1200 - WIFI5</t>
+  </si>
+  <si>
+    <t>NO BREAK INTELBRAS (600VA)</t>
+  </si>
+  <si>
+    <t>NO BREAK INTELBRAS (700VA)</t>
+  </si>
+  <si>
+    <t>NO BREAK NHS (1.200VA)</t>
+  </si>
+  <si>
+    <t>NO BREAK SAARA (1.200VA)</t>
+  </si>
+  <si>
+    <t>NO BREAK INTELBRAS (1.200VA)</t>
+  </si>
+  <si>
+    <t>CÂMERAS INTELBRAS VIP BULLET</t>
+  </si>
+  <si>
+    <t>CÂMERAS INTELBRAS VIP DOME</t>
+  </si>
+  <si>
+    <t>CÂMERA BULLET INTELBRAS 1120B</t>
   </si>
 </sst>
 </file>
@@ -96,7 +456,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="\R\$\ #,##0.00"/>
   </numFmts>
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -119,6 +479,12 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF1B1C1D"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="3">
@@ -162,7 +528,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -174,7 +540,12 @@
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="1" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center" readingOrder="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -479,16 +850,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C10"/>
+  <dimension ref="A1:C256"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H7" sqref="H7"/>
+      <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="16.6640625" customWidth="1"/>
-    <col min="3" max="3" width="26.6640625" customWidth="1"/>
+    <col min="3" max="3" width="93.33203125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.3">
@@ -503,86 +874,1066 @@
       <c r="A2">
         <v>3569</v>
       </c>
-      <c r="C2" t="s">
-        <v>13</v>
+      <c r="C2" s="7" t="s">
+        <v>16</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>6402</v>
       </c>
-      <c r="C3" t="s">
-        <v>14</v>
-      </c>
+      <c r="C3" s="8"/>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>6403</v>
       </c>
-      <c r="C4" t="s">
-        <v>15</v>
+      <c r="C4" s="7" t="s">
+        <v>17</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>7135</v>
       </c>
-      <c r="C5" t="s">
-        <v>20</v>
-      </c>
+      <c r="C5" s="8"/>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>12858</v>
       </c>
-      <c r="C6" t="s">
-        <v>21</v>
+      <c r="C6" s="7" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>19864</v>
       </c>
-      <c r="C7" t="s">
-        <v>16</v>
-      </c>
+      <c r="C7" s="8"/>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>23239</v>
       </c>
-      <c r="C8" t="s">
-        <v>17</v>
+      <c r="C8" s="7" t="s">
+        <v>19</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="C9" t="s">
-        <v>18</v>
-      </c>
+      <c r="A9">
+        <v>13254</v>
+      </c>
+      <c r="C9" s="8"/>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="C10" t="s">
-        <v>19</v>
+      <c r="C10" s="7" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="C11" s="8"/>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="C12" s="7" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="C13" s="8"/>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="C14" s="7" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="C15" s="8"/>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="C16" s="7" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="17" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C17" s="8"/>
+    </row>
+    <row r="18" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C18" s="7" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="19" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C19" s="8"/>
+    </row>
+    <row r="20" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C20" s="7" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="21" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C21" s="8"/>
+    </row>
+    <row r="22" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C22" s="7" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="23" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C23" s="8"/>
+    </row>
+    <row r="24" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C24" s="7" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="25" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C25" s="8"/>
+    </row>
+    <row r="26" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C26" s="7" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="27" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C27" s="8"/>
+    </row>
+    <row r="28" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C28" s="7" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="29" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C29" s="8"/>
+    </row>
+    <row r="30" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C30" s="7" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="31" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C31" s="8"/>
+    </row>
+    <row r="32" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C32" s="7" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="33" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C33" s="8"/>
+    </row>
+    <row r="34" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C34" s="7" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="35" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C35" s="8"/>
+    </row>
+    <row r="36" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C36" s="7" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="37" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C37" s="8"/>
+    </row>
+    <row r="38" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C38" s="7" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="39" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C39" s="8"/>
+    </row>
+    <row r="40" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C40" s="7" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="41" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C41" s="8"/>
+    </row>
+    <row r="42" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C42" s="7" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="43" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C43" s="8"/>
+    </row>
+    <row r="44" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C44" s="7" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="45" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C45" s="8"/>
+    </row>
+    <row r="46" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C46" s="7" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="47" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C47" s="8"/>
+    </row>
+    <row r="48" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C48" s="7" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="49" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C49" s="8"/>
+    </row>
+    <row r="50" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C50" s="7" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="51" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C51" s="8"/>
+    </row>
+    <row r="52" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C52" s="7" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="53" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C53" s="8"/>
+    </row>
+    <row r="54" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C54" s="7" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="55" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C55" s="8"/>
+    </row>
+    <row r="56" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C56" s="7" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="57" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C57" s="8"/>
+    </row>
+    <row r="58" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C58" s="7" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="59" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C59" s="8"/>
+    </row>
+    <row r="60" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C60" s="7" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="61" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C61" s="8"/>
+    </row>
+    <row r="62" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C62" s="7" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="63" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C63" s="8"/>
+    </row>
+    <row r="64" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C64" s="7" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="65" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C65" s="8"/>
+    </row>
+    <row r="66" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C66" s="7" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="67" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C67" s="8"/>
+    </row>
+    <row r="68" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C68" s="7" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="69" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C69" s="8"/>
+    </row>
+    <row r="70" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C70" s="7" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="71" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C71" s="8"/>
+    </row>
+    <row r="72" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C72" s="7" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="73" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C73" s="8"/>
+    </row>
+    <row r="74" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C74" s="7" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="75" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C75" s="8"/>
+    </row>
+    <row r="76" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C76" s="7" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="77" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C77" s="8"/>
+    </row>
+    <row r="78" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C78" s="7" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="79" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C79" s="8"/>
+    </row>
+    <row r="80" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C80" s="7" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="81" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C81" s="8"/>
+    </row>
+    <row r="82" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C82" s="7" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="83" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C83" s="8"/>
+    </row>
+    <row r="84" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C84" s="7" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="85" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C85" s="8"/>
+    </row>
+    <row r="86" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C86" s="7" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="87" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C87" s="8"/>
+    </row>
+    <row r="88" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C88" s="7" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="89" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C89" s="8"/>
+    </row>
+    <row r="90" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C90" s="7" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="91" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C91" s="8"/>
+    </row>
+    <row r="92" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C92" s="7" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="93" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C93" s="8"/>
+    </row>
+    <row r="94" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C94" s="7" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="95" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C95" s="8"/>
+    </row>
+    <row r="96" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C96" s="7" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="97" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C97" s="8"/>
+    </row>
+    <row r="98" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C98" s="7" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="99" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C99" s="8"/>
+    </row>
+    <row r="100" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C100" s="7" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="101" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C101" s="8"/>
+    </row>
+    <row r="102" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C102" s="7" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="103" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C103" s="8"/>
+    </row>
+    <row r="104" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C104" s="7" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="105" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C105" s="8"/>
+    </row>
+    <row r="106" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C106" s="7" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="107" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C107" s="8"/>
+    </row>
+    <row r="108" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C108" s="7" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="109" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C109" s="8"/>
+    </row>
+    <row r="110" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C110" s="7" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="111" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C111" s="8"/>
+    </row>
+    <row r="112" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C112" s="7" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="113" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C113" s="8"/>
+    </row>
+    <row r="114" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C114" s="7" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="115" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C115" s="8"/>
+    </row>
+    <row r="116" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C116" s="7" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="117" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C117" s="8"/>
+    </row>
+    <row r="118" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C118" s="7" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="119" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C119" s="8"/>
+    </row>
+    <row r="120" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C120" s="7" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="121" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C121" s="8"/>
+    </row>
+    <row r="122" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C122" s="7" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="123" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C123" s="8"/>
+    </row>
+    <row r="124" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C124" s="7" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="125" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C125" s="8"/>
+    </row>
+    <row r="126" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C126" s="7" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="127" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C127" s="8"/>
+    </row>
+    <row r="128" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C128" s="7" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="129" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C129" s="8"/>
+    </row>
+    <row r="130" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C130" s="7" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="131" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C131" s="8"/>
+    </row>
+    <row r="132" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C132" s="7" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="133" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C133" s="8"/>
+    </row>
+    <row r="134" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C134" s="7" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="135" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C135" s="8"/>
+    </row>
+    <row r="136" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C136" s="7" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="137" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C137" s="8"/>
+    </row>
+    <row r="138" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C138" s="7" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="139" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C139" s="8"/>
+    </row>
+    <row r="140" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C140" s="7" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="141" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C141" s="8"/>
+    </row>
+    <row r="142" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C142" s="7" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="143" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C143" s="8"/>
+    </row>
+    <row r="144" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C144" s="7" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="145" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C145" s="8"/>
+    </row>
+    <row r="146" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C146" s="7" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="147" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C147" s="8"/>
+    </row>
+    <row r="148" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C148" s="7" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="149" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C149" s="8"/>
+    </row>
+    <row r="150" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C150" s="7" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="151" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C151" s="8"/>
+    </row>
+    <row r="152" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C152" s="7" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="153" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C153" s="8"/>
+    </row>
+    <row r="154" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C154" s="7" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="155" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C155" s="8"/>
+    </row>
+    <row r="156" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C156" s="7" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="157" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C157" s="8"/>
+    </row>
+    <row r="158" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C158" s="7" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="159" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C159" s="8"/>
+    </row>
+    <row r="160" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C160" s="7" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="161" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C161" s="8"/>
+    </row>
+    <row r="162" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C162" s="7" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="163" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C163" s="8"/>
+    </row>
+    <row r="164" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C164" s="7" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="165" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C165" s="8"/>
+    </row>
+    <row r="166" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C166" s="7" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="167" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C167" s="8"/>
+    </row>
+    <row r="168" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C168" s="7" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="169" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C169" s="8"/>
+    </row>
+    <row r="170" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C170" s="7" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="171" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C171" s="8"/>
+    </row>
+    <row r="172" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C172" s="7" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="173" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C173" s="8"/>
+    </row>
+    <row r="174" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C174" s="7" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="175" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C175" s="8"/>
+    </row>
+    <row r="176" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C176" s="7" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="177" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C177" s="8"/>
+    </row>
+    <row r="178" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C178" s="7" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="179" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C179" s="8"/>
+    </row>
+    <row r="180" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C180" s="7" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="181" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C181" s="8"/>
+    </row>
+    <row r="182" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C182" s="7" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="183" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C183" s="8"/>
+    </row>
+    <row r="184" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C184" s="7" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="185" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C185" s="8"/>
+    </row>
+    <row r="186" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C186" s="7" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="187" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C187" s="8"/>
+    </row>
+    <row r="188" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C188" s="7" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="189" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C189" s="8"/>
+    </row>
+    <row r="190" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C190" s="7" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="191" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C191" s="8"/>
+    </row>
+    <row r="192" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C192" s="7" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="193" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C193" s="8"/>
+    </row>
+    <row r="194" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C194" s="7" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="195" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C195" s="8"/>
+    </row>
+    <row r="196" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C196" s="7" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="197" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C197" s="8"/>
+    </row>
+    <row r="198" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C198" s="7" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="199" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C199" s="8"/>
+    </row>
+    <row r="200" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C200" s="7" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="201" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C201" s="8"/>
+    </row>
+    <row r="202" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C202" s="7" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="203" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C203" s="8"/>
+    </row>
+    <row r="204" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C204" s="7" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="205" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C205" s="8"/>
+    </row>
+    <row r="206" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C206" s="7" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="207" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C207" s="8"/>
+    </row>
+    <row r="208" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C208" s="7" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="209" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C209" s="8"/>
+    </row>
+    <row r="210" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C210" s="7" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="211" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C211" s="8"/>
+    </row>
+    <row r="212" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C212" s="7" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="213" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C213" s="8"/>
+    </row>
+    <row r="214" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C214" s="7" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="215" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C215" s="8"/>
+    </row>
+    <row r="216" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C216" s="7" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="217" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C217" s="8"/>
+    </row>
+    <row r="218" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C218" s="7" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="219" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C219" s="8"/>
+    </row>
+    <row r="220" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C220" s="7" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="221" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C221" s="8"/>
+    </row>
+    <row r="222" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C222" s="7" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="223" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C223" s="8"/>
+    </row>
+    <row r="224" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C224" s="7" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="225" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C225" s="8"/>
+    </row>
+    <row r="226" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C226" s="7" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="227" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C227" s="8"/>
+    </row>
+    <row r="228" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C228" s="7" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="229" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C229" s="8"/>
+    </row>
+    <row r="230" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C230" s="7" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="231" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C231" s="8"/>
+    </row>
+    <row r="232" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C232" s="7" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="233" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C233" s="8"/>
+    </row>
+    <row r="234" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C234" s="7" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="235" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C235" s="8"/>
+    </row>
+    <row r="236" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C236" s="7" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="237" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C237" s="8"/>
+    </row>
+    <row r="238" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C238" s="7" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="239" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C239" s="8"/>
+    </row>
+    <row r="240" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C240" s="7" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="241" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C241" s="8"/>
+    </row>
+    <row r="242" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C242" s="7" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="243" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C243" s="8"/>
+    </row>
+    <row r="244" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C244" s="7" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="245" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C245" s="8"/>
+    </row>
+    <row r="246" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C246" s="7" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="247" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C247" s="8"/>
+    </row>
+    <row r="248" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C248" s="7" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="249" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C249" s="8"/>
+    </row>
+    <row r="250" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C250" s="7" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="251" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C251" s="8"/>
+    </row>
+    <row r="252" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C252" s="7" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="253" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C253" s="8"/>
+    </row>
+    <row r="254" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C254" s="7" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="255" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C255" s="8"/>
+    </row>
+    <row r="256" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C256" s="7" t="s">
+        <v>93</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E14"/>
+  <dimension ref="A1:E21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="J22" sqref="J22"/>
+      <selection pane="bottomLeft" activeCell="I14" sqref="I14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="16.6640625" customWidth="1"/>
-    <col min="2" max="2" width="26.6640625" customWidth="1"/>
+    <col min="2" max="2" width="51" customWidth="1"/>
     <col min="3" max="3" width="14.6640625" style="2" customWidth="1"/>
     <col min="4" max="5" width="16.6640625" style="3" customWidth="1"/>
   </cols>
@@ -595,102 +1946,354 @@
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>4</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>5</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2">
-        <v>3569</v>
+        <v>13254</v>
       </c>
       <c r="B2" t="s">
-        <v>2</v>
+        <v>125</v>
       </c>
       <c r="C2" s="2">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="D2" s="3">
+        <v>2500</v>
+      </c>
+      <c r="E2" s="3">
         <v>2000</v>
-      </c>
-      <c r="E2" s="3">
-        <v>2300</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3">
-        <v>7135</v>
+        <v>13254</v>
       </c>
       <c r="B3" t="s">
-        <v>16</v>
+        <v>127</v>
       </c>
       <c r="C3" s="2">
         <v>2</v>
       </c>
       <c r="D3" s="3">
-        <v>15</v>
+        <v>300</v>
       </c>
       <c r="E3" s="3">
-        <v>30</v>
+        <v>220</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4">
-        <v>3569</v>
+        <v>13254</v>
       </c>
       <c r="B4" t="s">
-        <v>17</v>
+        <v>93</v>
       </c>
       <c r="C4" s="2">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="D4" s="3">
-        <v>500</v>
+        <v>1000</v>
       </c>
       <c r="E4" s="3">
-        <v>550</v>
+        <v>650</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5">
-        <v>19864</v>
+        <v>13254</v>
       </c>
       <c r="B5" t="s">
-        <v>18</v>
+        <v>72</v>
       </c>
       <c r="C5" s="2">
         <v>2</v>
       </c>
       <c r="D5" s="3">
-        <v>3000</v>
+        <v>1000</v>
       </c>
       <c r="E5" s="3">
-        <v>3200</v>
+        <v>650</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A6">
-        <v>19864</v>
+        <v>13254</v>
       </c>
       <c r="B6" t="s">
-        <v>14</v>
+        <v>104</v>
       </c>
       <c r="C6" s="2">
+        <v>1</v>
+      </c>
+      <c r="D6" s="3">
+        <v>1000</v>
+      </c>
+      <c r="E6" s="3">
+        <v>650</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A7">
+        <v>13254</v>
+      </c>
+      <c r="B7" t="s">
+        <v>34</v>
+      </c>
+      <c r="C7" s="2">
+        <v>1</v>
+      </c>
+      <c r="D7" s="3">
+        <v>1000</v>
+      </c>
+      <c r="E7" s="3">
+        <v>650</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A8">
+        <v>13254</v>
+      </c>
+      <c r="B8" t="s">
+        <v>35</v>
+      </c>
+      <c r="C8" s="2">
+        <v>1</v>
+      </c>
+      <c r="D8" s="3">
+        <v>1000</v>
+      </c>
+      <c r="E8" s="3">
+        <v>650</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A9">
+        <v>13254</v>
+      </c>
+      <c r="B9" t="s">
+        <v>128</v>
+      </c>
+      <c r="C9" s="2">
+        <v>1</v>
+      </c>
+      <c r="D9" s="3">
+        <v>1000</v>
+      </c>
+      <c r="E9" s="3">
+        <v>650</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A10">
+        <v>13254</v>
+      </c>
+      <c r="B10" t="s">
+        <v>133</v>
+      </c>
+      <c r="C10" s="2">
+        <v>2</v>
+      </c>
+      <c r="D10" s="3">
+        <v>1000</v>
+      </c>
+      <c r="E10" s="3">
+        <v>650</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A11">
+        <v>13254</v>
+      </c>
+      <c r="B11" t="s">
+        <v>59</v>
+      </c>
+      <c r="C11" s="2">
+        <v>2</v>
+      </c>
+      <c r="D11" s="3">
+        <v>1000</v>
+      </c>
+      <c r="E11" s="3">
+        <v>650</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A12">
+        <v>13254</v>
+      </c>
+      <c r="B12" t="s">
+        <v>63</v>
+      </c>
+      <c r="C12" s="2">
+        <v>1</v>
+      </c>
+      <c r="D12" s="3">
+        <v>1000</v>
+      </c>
+      <c r="E12" s="3">
+        <v>650</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A13">
+        <v>13254</v>
+      </c>
+      <c r="B13" t="s">
+        <v>61</v>
+      </c>
+      <c r="C13" s="2">
+        <v>1</v>
+      </c>
+      <c r="D13" s="3">
+        <v>1000</v>
+      </c>
+      <c r="E13" s="3">
+        <v>650</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A14">
+        <v>13254</v>
+      </c>
+      <c r="B14" t="s">
+        <v>22</v>
+      </c>
+      <c r="C14" s="2">
         <v>3</v>
       </c>
-      <c r="D6" s="3">
-        <v>4200</v>
-      </c>
-      <c r="E6" s="3">
-        <v>5000</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="C14" s="7"/>
+      <c r="D14" s="3">
+        <v>1000</v>
+      </c>
+      <c r="E14" s="3">
+        <v>650</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A15">
+        <v>13254</v>
+      </c>
+      <c r="B15" t="s">
+        <v>108</v>
+      </c>
+      <c r="C15" s="2">
+        <v>7</v>
+      </c>
+      <c r="D15" s="3">
+        <v>1000</v>
+      </c>
+      <c r="E15" s="3">
+        <v>650</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A16">
+        <v>13254</v>
+      </c>
+      <c r="B16" t="s">
+        <v>21</v>
+      </c>
+      <c r="C16" s="2">
+        <v>25</v>
+      </c>
+      <c r="D16" s="3">
+        <v>1000</v>
+      </c>
+      <c r="E16" s="3">
+        <v>650</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A17">
+        <v>13254</v>
+      </c>
+      <c r="B17" t="s">
+        <v>121</v>
+      </c>
+      <c r="C17" s="2">
+        <v>1</v>
+      </c>
+      <c r="D17" s="3">
+        <v>1000</v>
+      </c>
+      <c r="E17" s="3">
+        <v>650</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A18">
+        <v>13254</v>
+      </c>
+      <c r="B18" t="s">
+        <v>13</v>
+      </c>
+      <c r="C18" s="2">
+        <v>1</v>
+      </c>
+      <c r="D18" s="3">
+        <v>1000</v>
+      </c>
+      <c r="E18" s="3">
+        <v>650</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A19">
+        <v>13254</v>
+      </c>
+      <c r="B19" t="s">
+        <v>106</v>
+      </c>
+      <c r="C19" s="2">
+        <v>2</v>
+      </c>
+      <c r="D19" s="3">
+        <v>1000</v>
+      </c>
+      <c r="E19" s="3">
+        <v>650</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A20">
+        <v>13254</v>
+      </c>
+      <c r="B20" t="s">
+        <v>132</v>
+      </c>
+      <c r="C20" s="2">
+        <v>1</v>
+      </c>
+      <c r="D20" s="3">
+        <v>1000</v>
+      </c>
+      <c r="E20" s="3">
+        <v>650</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A21">
+        <v>13254</v>
+      </c>
+      <c r="B21" t="s">
+        <v>99</v>
+      </c>
+      <c r="C21" s="2">
+        <v>1</v>
+      </c>
+      <c r="D21" s="3">
+        <v>1000</v>
+      </c>
+      <c r="E21" s="3">
+        <v>650</v>
+      </c>
     </row>
   </sheetData>
   <dataValidations count="2">
@@ -702,19 +2305,18 @@
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="2">
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
-            <xm:f>Listas!$A$2:$A$1000</xm:f>
+            <xm:f>Listas!$A$2:$A$993</xm:f>
           </x14:formula1>
-          <xm:sqref>A2:A10002</xm:sqref>
+          <xm:sqref>A21:A10002 A2:A19</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
-            <xm:f>Listas!$C$2:$C$1000</xm:f>
+            <xm:f>Listas!$C$2:$C$993</xm:f>
           </x14:formula1>
           <xm:sqref>B2:B10002</xm:sqref>
         </x14:dataValidation>
@@ -739,37 +2341,37 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" s="5" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" s="4" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" s="4" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" s="4" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5" s="4" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A6" s="4" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A7" s="4" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.3">

</xml_diff>